<commit_message>
Updated benchmarks docs x2
</commit_message>
<xml_diff>
--- a/tests/results/test-firegex.xlsx
+++ b/tests/results/test-firegex.xlsx
@@ -5,75 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domysh/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/domysh/repos/firegex/tests/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E56F8B96-EC1F-CA47-98C2-821B9CA59238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9311A56B-5BBB-D94C-9E9C-4E7B6EDAE60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20100" xr2:uid="{06A715B8-6EAB-1F4E-A0F8-BDDBE17B8663}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Foglio1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Foglio1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Foglio1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Foglio1!$A$1</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Foglio1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Foglio1!$A$1</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Foglio1!$A$2:$A$52</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Foglio1!$B$1</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Foglio1!$B$2:$B$52</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Foglio1!$C$1</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Foglio1!$C$2:$C$52</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Foglio1!$D$1</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Foglio1!$D$2:$D$52</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Foglio1!$E$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Foglio1!$E$2:$E$52</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Foglio1!$A$2:$A$52</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,21 +123,25 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mj-lt"/>
-                <a:ea typeface="+mj-ea"/>
-                <a:cs typeface="+mj-cs"/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT"/>
-              <a:t>Firegex benchmark</a:t>
+              <a:rPr lang="it-IT" sz="2400" b="1"/>
+              <a:t>Firegex</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="it-IT" sz="2400" b="1" baseline="0"/>
+              <a:t> Benchmark</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -213,16 +159,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="it-IT"/>
@@ -231,7 +177,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8213364612594209E-2"/>
+          <c:y val="0.14555624117369972"/>
+          <c:w val="0.880623749181775"/>
+          <c:h val="0.70387271434569942"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -250,7 +206,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -588,7 +544,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-089D-1A41-8BCB-3A4C702658CF}"/>
+              <c16:uniqueId val="{00000000-E86A-5A4D-B47C-CC660FC1E485}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -607,7 +563,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -945,7 +901,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-089D-1A41-8BCB-3A4C702658CF}"/>
+              <c16:uniqueId val="{00000001-E86A-5A4D-B47C-CC660FC1E485}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -964,7 +920,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1302,7 +1258,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-089D-1A41-8BCB-3A4C702658CF}"/>
+              <c16:uniqueId val="{00000002-E86A-5A4D-B47C-CC660FC1E485}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1321,7 +1277,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -1659,7 +1615,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-089D-1A41-8BCB-3A4C702658CF}"/>
+              <c16:uniqueId val="{00000003-E86A-5A4D-B47C-CC660FC1E485}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1672,17 +1628,17 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1450513120"/>
-        <c:axId val="1582165696"/>
+        <c:axId val="774619232"/>
+        <c:axId val="774620960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1450513120"/>
+        <c:axId val="774619232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1696,81 +1652,6 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1582165696"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1582165696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1794,66 +1675,68 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1450513120"/>
+        <c:crossAx val="774620960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="774620960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="774619232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="hundreds"/>
-          <c:dispUnitsLbl>
-            <c:tx>
-              <c:rich>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:r>
-                    <a:rPr lang="it-IT"/>
-                    <a:t>MB/s</a:t>
-                  </a:r>
-                </a:p>
-              </c:rich>
-            </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
-              </a:p>
-            </c:txPr>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1864,7 +1747,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1914,7 +1797,7 @@
     <a:effectLst/>
   </c:spPr>
   <c:txPr>
-    <a:bodyPr/>
+    <a:bodyPr rot="0" vert="horz"/>
     <a:lstStyle/>
     <a:p>
       <a:pPr>
@@ -1928,6 +1811,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1972,7 +1856,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="235">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1983,7 +1867,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2006,14 +1890,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2029,7 +1913,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2049,17 +1933,22 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2068,12 +1957,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2083,12 +1972,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2100,13 +1989,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="38100" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2115,29 +2004,36 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="8"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2159,13 +2055,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2180,15 +2078,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2199,17 +2097,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2218,14 +2116,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2237,15 +2135,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2264,7 +2168,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2283,17 +2187,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2302,16 +2206,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2332,7 +2237,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -2340,7 +2245,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2353,17 +2258,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2371,10 +2265,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2389,13 +2283,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="major">
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="2000" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2404,14 +2298,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2441,8 +2335,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2465,8 +2359,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2476,22 +2376,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>74911</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123752</xdr:rowOff>
+      <xdr:colOff>383822</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>150989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>563384</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>200525</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>155221</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Grafico 1">
+        <xdr:cNvPr id="3" name="Grafico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58FF19AE-EB20-7048-B045-3EDEE6F2B858}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C916C86-1056-B050-5EED-9FD1E4C3AFED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2510,6 +2410,136 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.62598</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.06306</cdr:x>
+      <cdr:y>0.65551</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="CasellaDiTesto 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1454BD90-6308-7374-FC74-39D635C2BD71}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="2692399"/>
+          <a:ext cx="416278" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="it-IT" sz="1100" kern="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00641</cdr:x>
+      <cdr:y>0.42257</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.03848</cdr:x>
+      <cdr:y>0.53412</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="CasellaDiTesto 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12D13948-377D-F59F-BF39-BA464DDF6134}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-91720" y="1951565"/>
+          <a:ext cx="479778" cy="211667"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="it-IT" sz="900" kern="1200"/>
+            <a:t>MB/s</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.46558</cdr:x>
+      <cdr:y>0.89501</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.72745</cdr:x>
+      <cdr:y>0.95735</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="CasellaDiTesto 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E87CEA94-FB21-E551-BB28-8C4EEB06EF3B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3073400" y="3849511"/>
+          <a:ext cx="1728611" cy="268112"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="it-IT" sz="800" kern="1200"/>
+            <a:t>N.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="800" kern="1200" baseline="0"/>
+            <a:t> of regexes</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="800" kern="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2831,8 +2861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6121C1B-CDBB-4649-9DD2-9D2E4AE1EF2E}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>